<commit_message>
Dicionario de dados exemplo finalizado
</commit_message>
<xml_diff>
--- a/Projeto Pratico/Dicionario de Dados/Dicionario de Dados - DB_Faculdade.xlsx
+++ b/Projeto Pratico/Dicionario de Dados/Dicionario de Dados - DB_Faculdade.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3C7B873E-B413-4167-BD5B-F8F9DA0779F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E161CA73-7C6D-4731-B81F-705265368C9D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Relacionamentos" sheetId="1" r:id="rId1"/>
+    <sheet name="Entidades" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="68">
   <si>
     <t>Dicionário de Dados</t>
   </si>
@@ -128,13 +129,109 @@
   </si>
   <si>
     <t>Tabela associativa ente Professor e Disciplina</t>
+  </si>
+  <si>
+    <t>Entidade Departamento</t>
+  </si>
+  <si>
+    <t>Atributos</t>
+  </si>
+  <si>
+    <t>Tipo de Dados</t>
+  </si>
+  <si>
+    <t>Comprimento</t>
+  </si>
+  <si>
+    <t>Cod_Departamento</t>
+  </si>
+  <si>
+    <t>Nome_Departamento</t>
+  </si>
+  <si>
+    <t>Inteiro</t>
+  </si>
+  <si>
+    <t>Caractere</t>
+  </si>
+  <si>
+    <t>4 bytes</t>
+  </si>
+  <si>
+    <t>40 bytes</t>
+  </si>
+  <si>
+    <t>PK, NOT NULL</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>Cod. De identificação do Departamento</t>
+  </si>
+  <si>
+    <t>Nome do deparatamento</t>
+  </si>
+  <si>
+    <t>Entidade Professor</t>
+  </si>
+  <si>
+    <t>Cod_Professor</t>
+  </si>
+  <si>
+    <t>Nome_Professor</t>
+  </si>
+  <si>
+    <t>Sobrenome_Professor</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Booleano</t>
+  </si>
+  <si>
+    <t>1 bit</t>
+  </si>
+  <si>
+    <t>FK, NOT NULL</t>
+  </si>
+  <si>
+    <t>Código de identificação do Professor</t>
+  </si>
+  <si>
+    <t>Nome do Professor</t>
+  </si>
+  <si>
+    <t>Sobrenome do Professor</t>
+  </si>
+  <si>
+    <t>Código de identificação do Departamento</t>
+  </si>
+  <si>
+    <t>Status do professor (lecionando/não lecionando)</t>
+  </si>
+  <si>
+    <t>Entidade Curso</t>
+  </si>
+  <si>
+    <t>Cod_Curso</t>
+  </si>
+  <si>
+    <t>Nome_Curso</t>
+  </si>
+  <si>
+    <t>Restrições</t>
+  </si>
+  <si>
+    <t>Código de identificação do Curso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,8 +269,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,8 +301,19 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -559,15 +674,198 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -598,28 +896,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -628,6 +944,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -646,19 +974,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -667,83 +1001,143 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="34" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="35" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="20% - Ênfase1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% - Ênfase2" xfId="5" builtinId="34"/>
     <cellStyle name="20% - Ênfase4" xfId="3" builtinId="42"/>
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutro" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1022,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I26"/>
+  <dimension ref="B1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,382 +1433,386 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="18"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
     </row>
     <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="43"/>
+      <c r="F5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="17" t="s">
+      <c r="G5" s="43"/>
+      <c r="H5" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="18"/>
+      <c r="I5" s="43"/>
     </row>
     <row r="6" spans="2:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="28"/>
+      <c r="F6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="7" t="s">
+      <c r="G6" s="21"/>
+      <c r="H6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="2:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15" t="s">
+      <c r="E7" s="33"/>
+      <c r="F7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="40" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="38" t="s">
+      <c r="E9" s="25"/>
+      <c r="F9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="44" t="s">
+      <c r="G9" s="27"/>
+      <c r="H9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="45"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="42" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="48" t="s">
+      <c r="E10" s="23"/>
+      <c r="F10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="47"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="28"/>
+      <c r="F11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="7" t="s">
+      <c r="G11" s="21"/>
+      <c r="H11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="8"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="2:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="28" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="35" t="s">
+      <c r="E13" s="28"/>
+      <c r="F13" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="7" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="8"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="34" t="s">
+      <c r="B14" s="44"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="36" t="s">
+      <c r="E14" s="52"/>
+      <c r="F14" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="49"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="34" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="36" t="s">
+      <c r="E15" s="52"/>
+      <c r="F15" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="49"/>
     </row>
     <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="29" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="37" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="G16" s="10"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="28" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="35" t="s">
+      <c r="E17" s="28"/>
+      <c r="F17" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="7" t="s">
+      <c r="G17" s="21"/>
+      <c r="H17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="34" t="s">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="44"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="36" t="s">
+      <c r="E18" s="52"/>
+      <c r="F18" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="34" t="s">
+      <c r="G18" s="34"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="49"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="44"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="36" t="s">
+      <c r="E19" s="52"/>
+      <c r="F19" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="33"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="29" t="s">
+      <c r="G19" s="34"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49"/>
+    </row>
+    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="37" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="50" t="s">
+      <c r="G20" s="10"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="51"/>
+      <c r="C21" s="2"/>
       <c r="D21" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="56" t="s">
+      <c r="E21" s="25"/>
+      <c r="F21" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="39"/>
-      <c r="H21" s="44" t="s">
+      <c r="G21" s="27"/>
+      <c r="H21" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="45"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="52"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="55" t="s">
+      <c r="I21" s="18"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="49"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="47"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="50" t="s">
+      <c r="G22" s="16"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="20"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="51"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="56" t="s">
+      <c r="E23" s="25"/>
+      <c r="F23" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="G23" s="39"/>
-      <c r="H23" s="44" t="s">
+      <c r="G23" s="27"/>
+      <c r="H23" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I23" s="45"/>
-    </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="52"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="55" t="s">
+      <c r="I23" s="18"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="43"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="49"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="47"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="s">
+      <c r="G24" s="16"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="20"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="51"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="56" t="s">
+      <c r="E25" s="25"/>
+      <c r="F25" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="39"/>
-      <c r="H25" s="44" t="s">
+      <c r="G25" s="27"/>
+      <c r="H25" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="I25" s="45"/>
-    </row>
-    <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="52"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="55" t="s">
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="43"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="49"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="47"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="20"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="64">
@@ -1430,22 +1828,22 @@
     <mergeCell ref="H23:I24"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B17:C20"/>
     <mergeCell ref="B21:C22"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B17:C20"/>
     <mergeCell ref="H17:I20"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="B2:I3"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B13:C16"/>
@@ -1486,4 +1884,414 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F67FD7C-D84F-456E-805B-C68ED7990EB9}">
+  <dimension ref="B1:J19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="43"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="43"/>
+      <c r="F3" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="43"/>
+      <c r="I3" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="70"/>
+    </row>
+    <row r="4" spans="2:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="77" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="78"/>
+      <c r="D4" s="80" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="80"/>
+      <c r="F4" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="82"/>
+      <c r="I4" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="64"/>
+    </row>
+    <row r="5" spans="2:10" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="81"/>
+      <c r="F5" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="83"/>
+      <c r="I5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="73"/>
+    </row>
+    <row r="8" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="73"/>
+      <c r="D8" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="73"/>
+      <c r="F8" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="73"/>
+      <c r="I8" s="71" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="73"/>
+    </row>
+    <row r="9" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="84" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="80" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="80"/>
+      <c r="F9" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="82"/>
+      <c r="I9" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="64"/>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="85" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="86"/>
+      <c r="D10" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="90"/>
+      <c r="F10" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="92" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="92"/>
+      <c r="I10" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="66"/>
+    </row>
+    <row r="11" spans="2:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="86"/>
+      <c r="D11" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="90"/>
+      <c r="F11" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="92" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="92"/>
+      <c r="I11" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" spans="2:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="85" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="86"/>
+      <c r="D12" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="90"/>
+      <c r="F12" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="92"/>
+      <c r="I12" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="30"/>
+    </row>
+    <row r="13" spans="2:10" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="81"/>
+      <c r="F13" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="83"/>
+      <c r="I13" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+    </row>
+    <row r="15" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="73"/>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="74" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="75"/>
+      <c r="D16" s="74" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="75"/>
+      <c r="F16" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="75"/>
+      <c r="I16" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="75"/>
+    </row>
+    <row r="17" spans="2:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="88" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="91"/>
+      <c r="F17" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="93" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="93"/>
+      <c r="I17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="89" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="90"/>
+      <c r="F18" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="92" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="92"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="66"/>
+    </row>
+    <row r="19" spans="2:10" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="79" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="81"/>
+      <c r="F19" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="83"/>
+      <c r="I19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G18:H18"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>